<commit_message>
Complete code Change for the Configurable Pricing Feature
</commit_message>
<xml_diff>
--- a/ConfigurablePricing_TestData.xlsx
+++ b/ConfigurablePricing_TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Pricing" sheetId="1" state="visible" r:id="rId2"/>
@@ -14,7 +14,6 @@
     <sheet name="Order" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">Product!$15:$15</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">Product!$15:$15</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="41">
   <si>
     <t xml:space="preserve">admin</t>
   </si>
@@ -83,55 +82,31 @@
     <t xml:space="preserve">7</t>
   </si>
   <si>
-    <t xml:space="preserve">Web Data 20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Services</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Billing Product 1</t>
+    <t xml:space="preserve">Pricing category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pricing Product 1</t>
   </si>
   <si>
     <t xml:space="preserve">United States Dollar</t>
   </si>
   <si>
-    <t xml:space="preserve">Monthly</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Billing Product 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">One time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Billing Product 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Semi-monthly</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dependent Category</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Billing Category Product 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Billing Category Product 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Billing Category Product 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Billing Category Product 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Billing Category Product 5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Billing Category Product 6</t>
+    <t xml:space="preserve">Items</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plan Pricing Product1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plan Pricing Category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pricing Product 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plan Pricing Product 2</t>
   </si>
   <si>
     <t xml:space="preserve">Default</t>
@@ -143,28 +118,37 @@
     <t xml:space="preserve">Volume Pricing Customer</t>
   </si>
   <si>
-    <t xml:space="preserve">Leo Holder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pre paid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">William</t>
-  </si>
-  <si>
-    <t xml:space="preserve">post paid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Olivia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Isabella</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sophia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jacob</t>
+    <t xml:space="preserve">US$5.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US$7.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US$17.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US$21.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US$41.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US$57.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US$117.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US$62.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US$142.00</t>
   </si>
 </sst>
 </file>
@@ -289,20 +273,20 @@
   </sheetPr>
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H1" activeCellId="1" sqref="K2 H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.837037037037"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.2074074074074"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.0703703703704"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="16.9518518518519"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="16.1703703703704"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="6.07407407407407"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="4.73703703703704"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="1" width="14.3074074074074"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="16.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="16.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="6.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="4.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="1" width="14.31"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -375,7 +359,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -388,28 +372,30 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K2" activeCellId="0" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.9962962962963"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.4259259259259"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.462962962963"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="21.362962962963"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="31.4555555555556"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="28.6148148148148"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="7.54444444444444"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="16.1703703703704"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="19.1074074074074"/>
-    <col collapsed="false" hidden="false" max="1019" min="10" style="1" width="13.4259259259259"/>
-    <col collapsed="false" hidden="false" max="1025" min="1020" style="0" width="9.6037037037037"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="21.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="31.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="28.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="7.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="16.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="19.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="15.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="18.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1019" min="12" style="1" width="13.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1020" style="0" width="9.6"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -417,110 +403,68 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>22</v>
       </c>
       <c r="M1" s="4"/>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D2" s="0"/>
-      <c r="E2" s="1" t="s">
+    <row r="2" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D2" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="E2" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="G2" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D3" s="0"/>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H3" s="1" t="s">
+    </row>
+    <row r="4" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E4" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="H4" s="0"/>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E5" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H5" s="0"/>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E6" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H6" s="0"/>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E7" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E8" s="0"/>
-      <c r="G8" s="0"/>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E9" s="0"/>
-      <c r="G9" s="0"/>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E10" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E11" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>5</v>
-      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -528,7 +472,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -543,19 +487,19 @@
   </sheetPr>
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E13" activeCellId="1" sqref="K2 E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.4259259259259"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.9111111111111"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.2481481481481"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.8148148148148"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="29.0074074074074"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="24.3037037037037"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="13.4259259259259"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="18.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="29.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="24.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="1" width="13.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -566,21 +510,21 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E2" s="2" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -589,7 +533,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -602,28 +546,27 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="1" sqref="K2 C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.9740740740741"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="21.262962962963"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="19.2074074074074"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="14.6"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="17.737037037037"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="13.1296296296296"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="28.9074074074074"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="18.8148148148148"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="29.3"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="22.0481481481481"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="20.1851851851852"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="25.6740740740741"/>
-    <col collapsed="false" hidden="false" max="1022" min="13" style="1" width="13.4259259259259"/>
-    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="13.4259259259259"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="21.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="19.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="25.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="19.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="5.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="9.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="9.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="20.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="25.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1020" min="11" style="1" width="13.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1022" min="1021" style="0" width="13.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1023" style="0" width="8.36"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -634,85 +577,84 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>20</v>
+      <c r="E1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="19.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D3" s="2"/>
+      <c r="E3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D4" s="2"/>
+      <c r="E4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D3" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3" s="4"/>
-      <c r="G3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D4" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F4" s="4"/>
-      <c r="G4" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D5" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F5" s="4"/>
-      <c r="G5" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D6" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F6" s="4"/>
-      <c r="G6" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -721,7 +663,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
created order for TieredPricingCustomer and VolumePricingCustomer
</commit_message>
<xml_diff>
--- a/ConfigurablePricing_TestData.xlsx
+++ b/ConfigurablePricing_TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Pricing" sheetId="1" state="visible" r:id="rId2"/>
@@ -14,6 +14,7 @@
     <sheet name="Order" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">Product!$15:$15</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">Product!$15:$15</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
@@ -127,7 +128,7 @@
     <t xml:space="preserve">US$7.00</t>
   </si>
   <si>
-    <t xml:space="preserve">US$17.00</t>
+    <t xml:space="preserve">US$16.98</t>
   </si>
   <si>
     <t xml:space="preserve">US$21.00</t>
@@ -273,20 +274,20 @@
   </sheetPr>
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H1" activeCellId="1" sqref="K2 H1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="16.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="16.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="6.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="4.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="1" width="14.31"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.1296296296296"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.6962962962963"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.462962962963"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="17.2481481481481"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="16.5592592592593"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="6.17407407407407"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="4.8"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="1" width="14.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -359,7 +360,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -374,25 +375,25 @@
   </sheetPr>
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="K2" activeCellId="0" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="21.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="31.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="28.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="7.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="16.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="19.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="15.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="18.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1019" min="12" style="1" width="13.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1020" style="0" width="9.6"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.1925925925926"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.7185185185185"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.8555555555556"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="21.9518518518519"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="32.2407407407407"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="29.3"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="7.64444444444445"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="16.5592592592593"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="19.5"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="16.0703703703704"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="18.8148148148148"/>
+    <col collapsed="false" hidden="false" max="1019" min="12" style="1" width="13.7185185185185"/>
+    <col collapsed="false" hidden="false" max="1025" min="1020" style="0" width="9.8"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -459,6 +460,7 @@
       <c r="E3" s="2" t="s">
         <v>25</v>
       </c>
+      <c r="H3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E4" s="2" t="s">
@@ -472,7 +474,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -487,19 +489,19 @@
   </sheetPr>
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E13" activeCellId="1" sqref="K2 E13"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="18.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="29.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="24.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="1" width="13.43"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.7185185185185"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.3037037037037"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.6407407407407"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.2074074074074"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="29.6925925925926"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="24.8888888888889"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="13.7185185185185"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -533,7 +535,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -548,25 +550,25 @@
   </sheetPr>
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="1" sqref="K2 C1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.97"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="21.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="19.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="25.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="19.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="5.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="9.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="9.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="20.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="25.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1020" min="11" style="1" width="13.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1022" min="1021" style="0" width="13.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1023" style="0" width="8.36"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.2703703703704"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="21.8518518518519"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="19.6962962962963"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="25.7740740740741"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="19.9925925925926"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="5.58518518518519"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="9.6037037037037"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="9.8"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="20.6777777777778"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="26.3592592592593"/>
+    <col collapsed="false" hidden="false" max="1020" min="11" style="1" width="13.7185185185185"/>
+    <col collapsed="false" hidden="false" max="1022" min="1021" style="0" width="13.7185185185185"/>
+    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="8.52592592592593"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -663,7 +665,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Added Filter for Customer in the Specific Pricing Feature
</commit_message>
<xml_diff>
--- a/ConfigurablePricing_TestData.xlsx
+++ b/ConfigurablePricing_TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Pricing" sheetId="1" state="visible" r:id="rId2"/>
@@ -14,7 +14,6 @@
     <sheet name="Order" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">Product!$15:$15</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">Product!$15:$15</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
@@ -35,7 +34,7 @@
     <t xml:space="preserve">WebData@123</t>
   </si>
   <si>
-    <t xml:space="preserve">Web Data 12</t>
+    <t xml:space="preserve">Web Data 3</t>
   </si>
   <si>
     <t xml:space="preserve">Test Pricing</t>
@@ -274,20 +273,20 @@
   </sheetPr>
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.1296296296296"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.6962962962963"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.462962962963"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="17.2481481481481"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="16.5592592592593"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="6.17407407407407"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="4.8"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="1" width="14.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="17.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="16.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="6.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="4.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="1" width="14.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -360,7 +359,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -375,25 +374,25 @@
   </sheetPr>
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K2" activeCellId="0" sqref="K2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K2" activeCellId="1" sqref="C1 K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.1925925925926"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.7185185185185"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.8555555555556"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="21.9518518518519"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="32.2407407407407"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="29.3"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="7.64444444444445"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="16.5592592592593"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="19.5"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="16.0703703703704"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="18.8148148148148"/>
-    <col collapsed="false" hidden="false" max="1019" min="12" style="1" width="13.7185185185185"/>
-    <col collapsed="false" hidden="false" max="1025" min="1020" style="0" width="9.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="21.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="32.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="29.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="7.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="16.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="19.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="16.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="18.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1019" min="12" style="1" width="13.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1020" style="0" width="9.8"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -474,7 +473,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -489,19 +488,19 @@
   </sheetPr>
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E13" activeCellId="1" sqref="C1 E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.7185185185185"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.3037037037037"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.6407407407407"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.2074074074074"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="29.6925925925926"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="24.8888888888889"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="13.7185185185185"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="19.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="29.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="24.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="1" width="13.72"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -535,7 +534,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -550,25 +549,25 @@
   </sheetPr>
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.2703703703704"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="21.8518518518519"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="19.6962962962963"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="25.7740740740741"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="19.9925925925926"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="5.58518518518519"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="9.6037037037037"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="9.8"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="20.6777777777778"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="26.3592592592593"/>
-    <col collapsed="false" hidden="false" max="1020" min="11" style="1" width="13.7185185185185"/>
-    <col collapsed="false" hidden="false" max="1022" min="1021" style="0" width="13.7185185185185"/>
-    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="8.52592592592593"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="21.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="19.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="25.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="19.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="5.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="9.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="9.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="20.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="26.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1020" min="11" style="1" width="13.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1022" min="1021" style="0" width="13.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1023" style="0" width="8.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -665,7 +664,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Added Filter for Customer in the Discount Feature
</commit_message>
<xml_diff>
--- a/ConfigurablePricing_TestData.xlsx
+++ b/ConfigurablePricing_TestData.xlsx
@@ -34,7 +34,7 @@
     <t xml:space="preserve">WebData@123</t>
   </si>
   <si>
-    <t xml:space="preserve">Web Data 3</t>
+    <t xml:space="preserve">Web Data 5</t>
   </si>
   <si>
     <t xml:space="preserve">Test Pricing</t>
@@ -82,7 +82,7 @@
     <t xml:space="preserve">7</t>
   </si>
   <si>
-    <t xml:space="preserve">Pricing category</t>
+    <t xml:space="preserve">Configurable Pricing category</t>
   </si>
   <si>
     <t xml:space="preserve">Pricing Product 1</t>
@@ -97,7 +97,35 @@
     <t xml:space="preserve">Plan Pricing Product1</t>
   </si>
   <si>
-    <t xml:space="preserve">Plan Pricing Category</t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Plan </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Configurable</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Pricing Category</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Plan</t>
@@ -112,10 +140,66 @@
     <t xml:space="preserve">Default</t>
   </si>
   <si>
-    <t xml:space="preserve">Tiered Pricing Customer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Volume Pricing Customer</t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Tiered </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Configurable </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Pricing Customer</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Volume </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Configurable </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Pricing Customer</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">US$5.00</t>
@@ -159,7 +243,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -189,6 +273,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -274,7 +364,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -375,7 +465,7 @@
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K2" activeCellId="1" sqref="C1 K2"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -395,7 +485,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1020" style="0" width="9.8"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -489,7 +579,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E13" activeCellId="1" sqref="C1 E13"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -503,7 +593,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="1" width="13.72"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -523,7 +613,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E2" s="2" t="s">
         <v>29</v>
       </c>
@@ -570,7 +660,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1023" style="0" width="8.53"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="27.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -598,7 +688,7 @@
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
     </row>
-    <row r="2" customFormat="false" ht="19.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="29.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D2" s="2" t="s">
         <v>29</v>
       </c>

</xml_diff>